<commit_message>
Update my data scraping
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_XW.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_XW.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\egret\analyses\scrapeUSDAseedmanual\scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0513DFDC-BD56-4726-8F4C-3CE14529E87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936EBE91-BA6E-4021-8CCD-E3F59B1D66F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Meta" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="218">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -98,10 +98,6 @@
     <t>pretreatment</t>
   </si>
   <si>
-    <t>any pretreatment before the germination</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stratification_temp_C</t>
   </si>
   <si>
@@ -167,17 +163,9 @@
     <t>total_germination_percent</t>
   </si>
   <si>
-    <t>total germination percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>avg_germination_percent</t>
   </si>
   <si>
-    <t>averaged germination percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>samples</t>
   </si>
   <si>
@@ -188,10 +176,6 @@
     <t>germination_rate</t>
   </si>
   <si>
-    <t>germination rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>avg_germinative_energy_percent</t>
   </si>
   <si>
@@ -232,9 +216,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>germ_rate_days</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -342,26 +323,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>storage for 24 months</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage for 3 months</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage for 36 months</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage for 15 months</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage for 8 months</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Betula</t>
   </si>
   <si>
@@ -582,38 +543,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1 month dry storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 month moist storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 month dry storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 month moist storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 month dry storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 month moist storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 month dry storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 month moist storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>70.8 (2.2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -654,29 +583,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H2SO4 60 mins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H2SO4 75 mins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>albus var. laevigatus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H2SO4 20 mins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>orbiculatus</t>
   </si>
   <si>
-    <t>H2SO4 30 mins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Table 4</t>
   </si>
   <si>
@@ -875,6 +788,74 @@
   </si>
   <si>
     <t>14 to 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dry storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moist storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>any pretreatment before the germination (chemical, storage)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>germination_time_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_germination_percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total germination percentage (if it is germination percentage without any specification, data should go to this column)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg_germination_percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>averaged germination percentage (only enter here if it specify it's average germination percentage)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>germination ratec (only the percentage data)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>days of 50% germination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any information you think will be helpful for data cleaning later</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extra notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All the ranges should be entered as 'to', e.g.: "5-10" in the table should be entered as "5 to 10"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If it is a dash in the table, it is NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For cold stratification and warm stratification, if they specify in the table it is 0, I think we should enter them as 0 instead of leaving them as blank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -918,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -927,6 +908,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,23 +1189,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ28"/>
+  <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.08203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1330,159 +1312,195 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1493,15 +1511,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED3BA84-D2E9-405D-BF49-9376D8E16D09}">
-  <dimension ref="A1:AE126"/>
+  <dimension ref="A1:AD126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R53" sqref="R53"/>
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA116" sqref="AA116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="7" max="7" width="37.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.75" bestFit="1" customWidth="1"/>
@@ -1514,10 +1537,10 @@
     <col min="25" max="25" width="23.75" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="19.5" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="37" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,84 +1569,81 @@
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>253</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="N2">
         <v>30</v>
@@ -1638,18 +1658,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>253</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N3">
         <v>30</v>
@@ -1658,24 +1678,24 @@
         <v>20</v>
       </c>
       <c r="Q3" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="S3">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N4">
         <v>30</v>
@@ -1684,24 +1704,24 @@
         <v>20</v>
       </c>
       <c r="Q4" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="S4">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>253</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N5">
         <v>30</v>
@@ -1710,348 +1730,351 @@
         <v>20</v>
       </c>
       <c r="Q5" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="S5">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>277</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S6">
         <v>100</v>
       </c>
-      <c r="AD6">
+      <c r="AC6">
         <v>38.200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>277</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>277</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S8">
         <v>100</v>
       </c>
-      <c r="AD8">
+      <c r="AC8">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>277</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S9">
         <v>81.5</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>277</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S10">
         <v>92.3</v>
       </c>
-      <c r="AD10">
+      <c r="AC10">
         <v>47.6</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>277</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S11">
         <v>21.2</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>277</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
         <v>63</v>
       </c>
-      <c r="D12" t="s">
+      <c r="M12" t="s">
         <v>68</v>
-      </c>
-      <c r="M12" t="s">
-        <v>73</v>
       </c>
       <c r="S12">
         <v>94.6</v>
       </c>
-      <c r="AD12">
+      <c r="AC12">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>277</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
       <c r="M13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S13">
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>277</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S14">
         <v>85</v>
       </c>
-      <c r="AD14">
+      <c r="AC14">
         <v>49.2</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" t="s">
         <v>69</v>
-      </c>
-      <c r="M15" t="s">
-        <v>74</v>
       </c>
       <c r="S15">
         <v>12.2</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>277</v>
       </c>
       <c r="B16" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S16">
         <v>98.4</v>
       </c>
-      <c r="AD16">
+      <c r="AC16">
         <v>55.2</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>277</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S17">
         <v>13.4</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>277</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>277</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S19">
         <v>92.7</v>
       </c>
-      <c r="AD19">
+      <c r="AC19">
         <v>45.5</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>277</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S20">
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>287</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G21">
+        <v>131400</v>
       </c>
       <c r="I21" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="P21">
         <v>15</v>
@@ -2063,21 +2086,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>287</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1051000</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="P22">
         <v>15</v>
@@ -2089,24 +2115,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>287</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G23">
+        <v>131400</v>
       </c>
       <c r="I23" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="Q23">
         <v>28</v>
@@ -2118,24 +2147,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>287</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1051000</v>
       </c>
       <c r="I24" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="Q24">
         <v>28</v>
@@ -2147,24 +2179,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>287</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="G25">
+        <v>131400</v>
       </c>
       <c r="I25" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="S25">
         <v>0</v>
@@ -2173,24 +2208,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>287</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1577000</v>
       </c>
       <c r="I26" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="S26">
         <v>2</v>
@@ -2199,24 +2237,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>287</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="G27">
+        <v>131400</v>
       </c>
       <c r="I27" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="Q27">
         <v>112</v>
@@ -2228,24 +2269,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>287</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="G28">
+        <v>131400</v>
       </c>
       <c r="I28" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="Q28">
         <v>112</v>
@@ -2257,21 +2301,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>287</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="G29">
+        <v>131400</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="S29">
         <v>26</v>
@@ -2280,21 +2327,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>287</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="G30">
+        <v>657001</v>
       </c>
       <c r="I30" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="S30">
         <v>48</v>
@@ -2303,24 +2353,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>287</v>
       </c>
       <c r="B31" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="G31">
+        <v>350400</v>
       </c>
       <c r="I31" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="S31">
         <v>33</v>
@@ -2329,24 +2382,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>287</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="G32">
+        <v>350400</v>
       </c>
       <c r="I32" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="S32">
         <v>56</v>
@@ -2360,16 +2416,19 @@
         <v>287</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1051000</v>
       </c>
       <c r="I33" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="S33">
         <v>39</v>
@@ -2383,19 +2442,22 @@
         <v>287</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1051000</v>
       </c>
       <c r="I34" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="S34">
         <v>68</v>
@@ -2409,19 +2471,22 @@
         <v>287</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
         <v>76</v>
       </c>
-      <c r="D35" t="s">
-        <v>81</v>
+      <c r="G35">
+        <v>350400</v>
       </c>
       <c r="I35" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="S35">
         <v>42</v>
@@ -2435,19 +2500,22 @@
         <v>287</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="G36">
+        <v>350400</v>
       </c>
       <c r="I36" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="S36">
         <v>53</v>
@@ -2461,19 +2529,22 @@
         <v>287</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="G37">
+        <v>350400</v>
       </c>
       <c r="I37" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="S37">
         <v>50</v>
@@ -2487,16 +2558,19 @@
         <v>287</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1051000</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="S38">
         <v>41</v>
@@ -2510,19 +2584,22 @@
         <v>287</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1051000</v>
       </c>
       <c r="I39" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="S39">
         <v>69</v>
@@ -2536,16 +2613,16 @@
         <v>309</v>
       </c>
       <c r="B40" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L40">
         <v>30</v>
@@ -2560,7 +2637,7 @@
         <v>15</v>
       </c>
       <c r="R40" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="S40">
         <v>27</v>
@@ -2574,13 +2651,13 @@
         <v>309</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L41">
         <v>0</v>
@@ -2595,7 +2672,7 @@
         <v>20</v>
       </c>
       <c r="R41" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="S41">
         <v>59</v>
@@ -2609,13 +2686,13 @@
         <v>309</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="L42">
         <v>0</v>
@@ -2630,7 +2707,7 @@
         <v>20</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="S42">
         <v>18</v>
@@ -2644,19 +2721,19 @@
         <v>309</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L43" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="M43">
         <v>8</v>
@@ -2682,19 +2759,19 @@
         <v>309</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L44" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="N44">
         <v>30</v>
@@ -2714,16 +2791,16 @@
         <v>309</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -2752,19 +2829,19 @@
         <v>309</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L46" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="M46">
         <v>8</v>
@@ -2790,16 +2867,16 @@
         <v>309</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F47" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L47">
         <v>0</v>
@@ -2828,19 +2905,19 @@
         <v>309</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="L48" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="M48">
         <v>8</v>
@@ -2852,7 +2929,7 @@
         <v>15</v>
       </c>
       <c r="R48" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.3">
@@ -2860,16 +2937,16 @@
         <v>309</v>
       </c>
       <c r="B49" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" t="s">
         <v>89</v>
-      </c>
-      <c r="D49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" t="s">
-        <v>99</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -2892,19 +2969,19 @@
         <v>309</v>
       </c>
       <c r="B50" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="L50" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="M50">
         <v>8</v>
@@ -2913,7 +2990,7 @@
         <v>30</v>
       </c>
       <c r="U50" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.3">
@@ -2921,13 +2998,13 @@
         <v>309</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -2942,7 +3019,7 @@
         <v>20</v>
       </c>
       <c r="R51" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="S51">
         <v>36</v>
@@ -2956,19 +3033,19 @@
         <v>309</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="L52" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="M52">
         <v>8</v>
@@ -2994,16 +3071,16 @@
         <v>309</v>
       </c>
       <c r="B53" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L53" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="M53">
         <v>8</v>
@@ -3029,13 +3106,13 @@
         <v>309</v>
       </c>
       <c r="B54" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -3064,16 +3141,16 @@
         <v>309</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F55" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="M55">
         <v>20</v>
@@ -3099,13 +3176,13 @@
         <v>331</v>
       </c>
       <c r="B56" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K56">
         <v>14</v>
@@ -3122,13 +3199,13 @@
         <v>331</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K57">
         <v>30</v>
@@ -3145,13 +3222,13 @@
         <v>331</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C58" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="K58">
         <v>60</v>
@@ -3168,13 +3245,13 @@
         <v>331</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D59" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="N59">
         <v>20</v>
@@ -3186,7 +3263,7 @@
         <v>70</v>
       </c>
       <c r="T59" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="U59">
         <v>50</v>
@@ -3197,13 +3274,13 @@
         <v>331</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="N60">
         <v>27</v>
@@ -3215,7 +3292,7 @@
         <v>60</v>
       </c>
       <c r="T60" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="U60">
         <v>2</v>
@@ -3226,16 +3303,16 @@
         <v>395</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -3252,16 +3329,16 @@
         <v>395</v>
       </c>
       <c r="B62" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C62" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E62" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L62">
         <v>28</v>
@@ -3278,16 +3355,16 @@
         <v>395</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E63" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -3304,16 +3381,16 @@
         <v>395</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E64" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="L64">
         <v>28</v>
@@ -3325,21 +3402,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>395</v>
       </c>
       <c r="B65" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E65" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="L65">
         <v>0</v>
@@ -3351,21 +3428,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>395</v>
       </c>
       <c r="B66" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E66" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="L66">
         <v>28</v>
@@ -3377,18 +3454,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>395</v>
       </c>
       <c r="B67" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D67" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -3415,18 +3492,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>395</v>
       </c>
       <c r="B68" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C68" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -3453,18 +3530,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>395</v>
       </c>
       <c r="B69" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D69" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K69">
         <v>58</v>
@@ -3491,24 +3568,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>395</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D70" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="N70">
         <v>30</v>
@@ -3529,18 +3606,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>395</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D71" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -3567,379 +3644,379 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>411</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C72" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D72" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="P72">
         <v>3</v>
       </c>
-      <c r="AD72">
+      <c r="AC72">
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>411</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C73" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D73" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="Q73">
         <v>28</v>
       </c>
       <c r="AA73" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="AB73" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>411</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C74" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D74" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="P74">
         <v>3</v>
       </c>
-      <c r="AD74">
+      <c r="AC74">
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>411</v>
       </c>
       <c r="B75" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C75" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D75" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="Q75">
         <v>28</v>
       </c>
       <c r="AA75" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="AB75" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>411</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D76" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="P76">
         <v>3</v>
       </c>
-      <c r="AD76">
+      <c r="AC76">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>411</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C77" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D77" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="Q77">
         <v>28</v>
       </c>
       <c r="AA77" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="AB77" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>411</v>
       </c>
       <c r="B78" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D78" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="P78">
         <v>3</v>
       </c>
-      <c r="AD78">
+      <c r="AC78">
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>411</v>
       </c>
       <c r="B79" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C79" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D79" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="Q79">
         <v>28</v>
       </c>
       <c r="AA79" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="AB79" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>411</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C80" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D80" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="P80">
         <v>3</v>
       </c>
-      <c r="AD80">
+      <c r="AC80">
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>411</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C81" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" t="s">
         <v>118</v>
-      </c>
-      <c r="D81" t="s">
-        <v>128</v>
       </c>
       <c r="Q81">
         <v>28</v>
       </c>
       <c r="AA81" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="AB81" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>411</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" t="s">
         <v>118</v>
-      </c>
-      <c r="D82" t="s">
-        <v>128</v>
       </c>
       <c r="P82">
         <v>3</v>
       </c>
-      <c r="AD82">
+      <c r="AC82">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>411</v>
       </c>
       <c r="B83" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C83" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D83" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="Q83">
         <v>28</v>
       </c>
       <c r="AA83" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="AB83" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>411</v>
       </c>
       <c r="B84" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C84" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D84" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="P84">
         <v>3</v>
       </c>
-      <c r="AD84">
+      <c r="AC84">
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>411</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C85" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D85" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="Q85">
         <v>28</v>
       </c>
       <c r="AA85" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="AB85" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>411</v>
       </c>
       <c r="B86" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C86" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D86" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="P86">
         <v>3</v>
       </c>
-      <c r="AD86">
+      <c r="AC86">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>411</v>
       </c>
       <c r="B87" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C87" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="P87">
         <v>3</v>
       </c>
-      <c r="AD87">
+      <c r="AC87">
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>411</v>
       </c>
       <c r="B88" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C88" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D88" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="P88">
         <v>3</v>
       </c>
-      <c r="AD88">
+      <c r="AC88">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>751</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C89" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D89" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L89">
         <v>60</v>
@@ -3948,18 +4025,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>751</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C90" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D90" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L90">
         <v>90</v>
@@ -3968,18 +4045,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>751</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C91" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D91" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L91">
         <v>120</v>
@@ -3988,18 +4065,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>751</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D92" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L92">
         <v>160</v>
@@ -4008,18 +4085,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>751</v>
       </c>
       <c r="B93" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D93" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L93">
         <v>180</v>
@@ -4028,64 +4105,73 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1074</v>
       </c>
       <c r="B94" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C94" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D94" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G94">
+        <v>43800</v>
       </c>
       <c r="I94" t="s">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="S94" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1074</v>
       </c>
       <c r="B95" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C95" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D95" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G95">
+        <v>43800</v>
       </c>
       <c r="I95" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="S95" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1074</v>
       </c>
       <c r="B96" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C96" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D96" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G96">
+        <v>87600</v>
       </c>
       <c r="I96" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="S96" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.3">
@@ -4093,19 +4179,22 @@
         <v>1074</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C97" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D97" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G97">
+        <v>87600</v>
       </c>
       <c r="I97" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="S97" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.3">
@@ -4113,19 +4202,22 @@
         <v>1074</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C98" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D98" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G98">
+        <v>131400</v>
       </c>
       <c r="I98" t="s">
-        <v>151</v>
+        <v>202</v>
       </c>
       <c r="S98" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.3">
@@ -4133,19 +4225,22 @@
         <v>1074</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C99" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D99" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G99">
+        <v>131400</v>
       </c>
       <c r="I99" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
       <c r="S99" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
@@ -4153,19 +4248,22 @@
         <v>1074</v>
       </c>
       <c r="B100" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C100" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D100" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G100">
+        <v>175200</v>
       </c>
       <c r="I100" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="S100" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.3">
@@ -4173,19 +4271,22 @@
         <v>1074</v>
       </c>
       <c r="B101" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C101" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D101" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G101">
+        <v>175200</v>
       </c>
       <c r="I101" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="S101" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.3">
@@ -4193,16 +4294,19 @@
         <v>1081</v>
       </c>
       <c r="B102" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C102" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D102" t="s">
-        <v>164</v>
+        <v>146</v>
+      </c>
+      <c r="G102">
+        <v>60</v>
       </c>
       <c r="I102" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="K102">
         <v>60</v>
@@ -4219,16 +4323,19 @@
         <v>1081</v>
       </c>
       <c r="B103" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C103" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D103" t="s">
-        <v>164</v>
+        <v>146</v>
+      </c>
+      <c r="G103">
+        <v>75</v>
       </c>
       <c r="I103" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="K103">
         <v>20</v>
@@ -4245,16 +4352,19 @@
         <v>1081</v>
       </c>
       <c r="B104" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C104" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D104" t="s">
-        <v>167</v>
+        <v>147</v>
+      </c>
+      <c r="G104">
+        <v>20</v>
       </c>
       <c r="I104" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -4271,13 +4381,13 @@
         <v>1081</v>
       </c>
       <c r="B105" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C105" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D105" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="K105">
         <v>112</v>
@@ -4294,16 +4404,19 @@
         <v>1081</v>
       </c>
       <c r="B106" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C106" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D106" t="s">
-        <v>167</v>
+        <v>147</v>
+      </c>
+      <c r="G106">
+        <v>60</v>
       </c>
       <c r="I106" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="K106">
         <v>84</v>
@@ -4320,13 +4433,13 @@
         <v>1081</v>
       </c>
       <c r="B107" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C107" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D107" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="K107">
         <v>91</v>
@@ -4343,16 +4456,19 @@
         <v>1081</v>
       </c>
       <c r="B108" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C108" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D108" t="s">
-        <v>167</v>
+        <v>147</v>
+      </c>
+      <c r="G108">
+        <v>60</v>
       </c>
       <c r="I108" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="L108">
         <v>140</v>
@@ -4366,13 +4482,13 @@
         <v>1081</v>
       </c>
       <c r="B109" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C109" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D109" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="K109">
         <v>120</v>
@@ -4389,16 +4505,19 @@
         <v>1081</v>
       </c>
       <c r="B110" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C110" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D110" t="s">
-        <v>169</v>
+        <v>148</v>
+      </c>
+      <c r="G110" t="s">
+        <v>204</v>
       </c>
       <c r="I110" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="K110">
         <v>20</v>
@@ -4415,16 +4534,19 @@
         <v>1081</v>
       </c>
       <c r="B111" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C111" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="D111" t="s">
-        <v>169</v>
+        <v>148</v>
+      </c>
+      <c r="G111">
+        <v>30</v>
       </c>
       <c r="I111" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="K111">
         <v>120</v>
@@ -4441,19 +4563,19 @@
         <v>668</v>
       </c>
       <c r="B112" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C112" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D112" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="L112">
         <v>90</v>
       </c>
       <c r="S112" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.3">
@@ -4461,13 +4583,13 @@
         <v>668</v>
       </c>
       <c r="B113" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C113" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D113" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="K113">
         <v>28</v>
@@ -4484,13 +4606,13 @@
         <v>668</v>
       </c>
       <c r="B114" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C114" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D114" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="L114">
         <v>56</v>
@@ -4504,13 +4626,13 @@
         <v>668</v>
       </c>
       <c r="B115" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C115" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D115" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="L115">
         <v>119</v>
@@ -4524,22 +4646,22 @@
         <v>1166</v>
       </c>
       <c r="B116" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C116" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D116" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="K116" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="L116" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="Q116" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="T116">
         <v>32</v>
@@ -4553,13 +4675,13 @@
         <v>1166</v>
       </c>
       <c r="B117" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C117" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D117" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="K117">
         <v>150</v>
@@ -4582,19 +4704,19 @@
         <v>1166</v>
       </c>
       <c r="B118" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C118" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D118" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="K118" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="L118" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="Q118">
         <v>120</v>
@@ -4611,13 +4733,13 @@
         <v>1166</v>
       </c>
       <c r="B119" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C119" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D119" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="K119">
         <v>60</v>
@@ -4640,19 +4762,19 @@
         <v>1166</v>
       </c>
       <c r="B120" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C120" t="s">
+        <v>165</v>
+      </c>
+      <c r="D120" t="s">
+        <v>171</v>
+      </c>
+      <c r="K120" t="s">
+        <v>184</v>
+      </c>
+      <c r="L120" t="s">
         <v>187</v>
-      </c>
-      <c r="D120" t="s">
-        <v>193</v>
-      </c>
-      <c r="K120" t="s">
-        <v>206</v>
-      </c>
-      <c r="L120" t="s">
-        <v>209</v>
       </c>
       <c r="Q120">
         <v>60</v>
@@ -4669,22 +4791,22 @@
         <v>1166</v>
       </c>
       <c r="B121" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C121" t="s">
+        <v>165</v>
+      </c>
+      <c r="D121" t="s">
+        <v>172</v>
+      </c>
+      <c r="K121" t="s">
+        <v>183</v>
+      </c>
+      <c r="L121" t="s">
         <v>187</v>
       </c>
-      <c r="D121" t="s">
-        <v>194</v>
-      </c>
-      <c r="K121" t="s">
-        <v>205</v>
-      </c>
-      <c r="L121" t="s">
-        <v>209</v>
-      </c>
       <c r="Q121" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="T121">
         <v>75</v>
@@ -4698,22 +4820,22 @@
         <v>1166</v>
       </c>
       <c r="B122" t="s">
+        <v>151</v>
+      </c>
+      <c r="C122" t="s">
+        <v>165</v>
+      </c>
+      <c r="D122" t="s">
         <v>173</v>
       </c>
-      <c r="C122" t="s">
-        <v>187</v>
-      </c>
-      <c r="D122" t="s">
-        <v>195</v>
-      </c>
       <c r="K122" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="L122">
         <v>75</v>
       </c>
       <c r="Q122" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="T122">
         <v>69</v>
@@ -4727,16 +4849,16 @@
         <v>1182</v>
       </c>
       <c r="B123" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C123" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D123" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="F123" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="J123">
         <v>5</v>
@@ -4774,19 +4896,19 @@
         <v>1182</v>
       </c>
       <c r="B124" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D124" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="F124" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="I124" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="M124">
         <v>8</v>
@@ -4818,16 +4940,16 @@
         <v>1184</v>
       </c>
       <c r="B125" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C125" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="D125" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="F125" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="N125">
         <v>30</v>
@@ -4850,13 +4972,13 @@
         <v>1184</v>
       </c>
       <c r="B126" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C126" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="D126" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="N126">
         <v>38</v>

</xml_diff>

<commit_message>
Add two lines of new data
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_XW.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_XW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\egret\analyses\scrapeUSDAseedmanual\scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A082DBAC-D780-484E-963D-A52302FCB2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0E976-1247-4505-BE1C-06D6F94F168A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="5040" windowWidth="19350" windowHeight="5720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="225">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -869,6 +869,21 @@
   </si>
   <si>
     <t>germ_rate_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subcordata</t>
+  </si>
+  <si>
+    <t>Prunus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tomentosa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6 to 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1532,11 +1547,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED3BA84-D2E9-405D-BF49-9376D8E16D09}">
-  <dimension ref="A1:AF126"/>
+  <dimension ref="A1:AF128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5028,6 +5043,55 @@
         <v>65</v>
       </c>
     </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>885</v>
+      </c>
+      <c r="B127">
+        <v>6</v>
+      </c>
+      <c r="C127" t="s">
+        <v>222</v>
+      </c>
+      <c r="D127" t="s">
+        <v>221</v>
+      </c>
+      <c r="L127" t="s">
+        <v>224</v>
+      </c>
+      <c r="M127">
+        <v>90</v>
+      </c>
+      <c r="R127">
+        <v>100</v>
+      </c>
+      <c r="U127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>885</v>
+      </c>
+      <c r="B128">
+        <v>6</v>
+      </c>
+      <c r="C128" t="s">
+        <v>222</v>
+      </c>
+      <c r="D128" t="s">
+        <v>223</v>
+      </c>
+      <c r="L128" t="s">
+        <v>224</v>
+      </c>
+      <c r="M128" t="s">
+        <v>182</v>
+      </c>
+      <c r="U128">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>